<commit_message>
Few changes and deleted some files
</commit_message>
<xml_diff>
--- a/webdriver_rediff/BillingSuite.xlsx
+++ b/webdriver_rediff/BillingSuite.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>TestCases</t>
   </si>
@@ -26,9 +26,6 @@
     <t>Test1</t>
   </si>
   <si>
-    <t>Test3</t>
-  </si>
-  <si>
     <t>Test4</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>C65</t>
   </si>
   <si>
-    <t>AddStock</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
@@ -174,6 +168,9 @@
   </si>
   <si>
     <t>ViewBillTest</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -559,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,15 +576,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -595,26 +592,26 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -627,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -651,63 +648,63 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -715,87 +712,87 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -803,47 +800,47 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1"/>
     </row>
@@ -852,31 +849,31 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -884,94 +881,94 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>13</v>
       </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>16</v>
       </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="E26" t="s">
-        <v>20</v>
-      </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commited files on 23/06/2016
</commit_message>
<xml_diff>
--- a/webdriver_rediff/BillingSuite.xlsx
+++ b/webdriver_rediff/BillingSuite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
   <si>
     <t>TestCases</t>
   </si>
@@ -116,61 +116,13 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>Stock Name</t>
-  </si>
-  <si>
-    <t>HDFC Bank Ltd.</t>
-  </si>
-  <si>
-    <t>PurchaseDate</t>
-  </si>
-  <si>
-    <t>19/12/2013</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Tata Consultancy Services Ltd.</t>
-  </si>
-  <si>
-    <t>NTPC Ltd.</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>Mozilla</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>8/4/2016</t>
-  </si>
-  <si>
     <t>ViewBillTest</t>
   </si>
   <si>
-    <t>Test2</t>
+    <t>PaymentOptionsTest</t>
   </si>
 </sst>
 </file>
@@ -252,14 +204,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,12 +508,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -584,15 +535,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -622,15 +573,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -662,7 +613,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -690,7 +641,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -703,8 +654,8 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
+      <c r="A7" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -718,260 +669,221 @@
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>46</v>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G21" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="H21" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E22" t="s">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F22" t="s">
         <v>21</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="3" t="s">
-        <v>4</v>
+      <c r="H22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>26</v>
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to update test cases
</commit_message>
<xml_diff>
--- a/webdriver_rediff/BillingSuite.xlsx
+++ b/webdriver_rediff/BillingSuite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -508,7 +508,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
checked in new test cases with some changes
</commit_message>
<xml_diff>
--- a/webdriver_rediff/BillingSuite.xlsx
+++ b/webdriver_rediff/BillingSuite.xlsx
@@ -10,12 +10,12 @@
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>TestCases</t>
   </si>
@@ -123,6 +123,27 @@
   </si>
   <si>
     <t>PaymentOptionsTest</t>
+  </si>
+  <si>
+    <t>CreateBillingTicketTest</t>
+  </si>
+  <si>
+    <t>Account # For Billing Ticket</t>
+  </si>
+  <si>
+    <t>200069083</t>
+  </si>
+  <si>
+    <t>Billing ticket title</t>
+  </si>
+  <si>
+    <t>testtitle</t>
+  </si>
+  <si>
+    <t>What is issue</t>
+  </si>
+  <si>
+    <t>bill not generating</t>
   </si>
 </sst>
 </file>
@@ -204,13 +225,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,6 +587,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -573,20 +603,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -882,6 +912,51 @@
         <v>31</v>
       </c>
     </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made changes for demo
</commit_message>
<xml_diff>
--- a/webdriver_rediff/BillingSuite.xlsx
+++ b/webdriver_rediff/BillingSuite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,7 +560,7 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -568,7 +568,7 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>

</xml_diff>